<commit_message>
Added healthy rivers metrics
</commit_message>
<xml_diff>
--- a/tables/CA_strategy_dashboard_metrics_v1.2_Apr_2022.xlsx
+++ b/tables/CA_strategy_dashboard_metrics_v1.2_Apr_2022.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kklausmeyer.TNC\Documents\workspace\dashboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Users\kklausmeyer\Documents\workspace\dashboard\dashboard\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDAE608-7A8E-44B9-8B3C-3E95613D47A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1230" yWindow="3240" windowWidth="26775" windowHeight="14580" firstSheet="1" activeTab="1" xr2:uid="{86613900-E34B-45B3-B6BC-5C32F032CB78}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22830" windowHeight="9645" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="5" r:id="rId1"/>
@@ -21,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CA_strategy_outcomes!$D$1:$D$57</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,6 +32,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="221">
   <si>
     <t>Sheet</t>
   </si>
@@ -202,6 +202,9 @@
     <t>BAU rate of conversion = 52,000 acres/yr, 2025 progress = 2030 x 30%</t>
   </si>
   <si>
+    <t>320K avoided CV lands and farmland via greenprints relative to BAU, assuming 75% effectiveness; plus 30K acres  via connected lands, assuming 25% effectiveness, Includes old Sus Dev strategy + disaster resilience - Carrie wrote methods doc</t>
+  </si>
+  <si>
     <t>avoided emissions</t>
   </si>
   <si>
@@ -220,9 +223,24 @@
     <t>soil and veg conservation via avoided conversion above (cumulative)</t>
   </si>
   <si>
+    <t>wildlife corridors and crossings</t>
+  </si>
+  <si>
+    <t>crossing structures designed and funded</t>
+  </si>
+  <si>
     <t>land improved</t>
   </si>
   <si>
+    <t>crossing structures</t>
+  </si>
+  <si>
+    <t>was 3 crossing structures in October 2021 metrics sheet, 2025 was originally 'designed and funded' changed to 1 structure</t>
+  </si>
+  <si>
+    <t>decreased mortality</t>
+  </si>
+  <si>
     <t>energy</t>
   </si>
   <si>
@@ -244,9 +262,15 @@
     <t>get to 50% by 2030 = 27% increase from BAU</t>
   </si>
   <si>
+    <t xml:space="preserve">note this is not TNC alone; climate emissions reduction; with some portion creditable to TNC- assumes a 58.8 MMTco2e 2019 emissions from electricity sector and linear decrease to 29 at 2030- cumulatively reduction relative to flat BAU </t>
+  </si>
+  <si>
     <t>nature based solutions</t>
   </si>
   <si>
+    <t xml:space="preserve">avoided emissions and/or increased sequestration </t>
+  </si>
+  <si>
     <t>BAU</t>
   </si>
   <si>
@@ -274,6 +298,33 @@
     <t>coastal wetlands restoration</t>
   </si>
   <si>
+    <t>forests</t>
+  </si>
+  <si>
+    <t>planned &amp; permitted</t>
+  </si>
+  <si>
+    <t>2,400,000 acres</t>
+  </si>
+  <si>
+    <t>2025 = 35% of 2030 outcome</t>
+  </si>
+  <si>
+    <t>streamlining process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fuels reduction </t>
+  </si>
+  <si>
+    <t>37,000 acres/yr</t>
+  </si>
+  <si>
+    <t>125K acres / year * 10yrs</t>
+  </si>
+  <si>
+    <t>actual projects on the ground, on federal lands; reps a cumulative acreage via doubling of BAU rate of Rx fire and mech treatment, starting in 2022 (plus 2020-21)- BAU is 62k acres/yr</t>
+  </si>
+  <si>
     <t>Land</t>
   </si>
   <si>
@@ -298,33 +349,6 @@
     <t>includes fee and easement, e.g., via LENS, RDMapper…</t>
   </si>
   <si>
-    <t>forests</t>
-  </si>
-  <si>
-    <t>planned &amp; permitted</t>
-  </si>
-  <si>
-    <t>2,400,000 acres</t>
-  </si>
-  <si>
-    <t>2025 = 35% of 2030 outcome</t>
-  </si>
-  <si>
-    <t>streamlining process</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fuels reduction </t>
-  </si>
-  <si>
-    <t>37,000 acres/yr</t>
-  </si>
-  <si>
-    <t>125K acres / year * 10yrs</t>
-  </si>
-  <si>
-    <t>actual projects on the ground, on federal lands; reps a cumulative acreage via doubling of BAU rate of Rx fire and mech treatment, starting in 2022 (plus 2020-21)- BAU is 62k acres/yr</t>
-  </si>
-  <si>
     <t>land protection</t>
   </si>
   <si>
@@ -340,6 +364,9 @@
     <t>business as usual rate</t>
   </si>
   <si>
+    <t>within priority zones; of all actors; via influence, etc.</t>
+  </si>
+  <si>
     <t>protection by TNC</t>
   </si>
   <si>
@@ -403,6 +430,9 @@
     <t>6 islands</t>
   </si>
   <si>
+    <t>9 islands - California islands, double count with island biosec strategy</t>
+  </si>
+  <si>
     <t>kelp</t>
   </si>
   <si>
@@ -529,15 +559,27 @@
     <t xml:space="preserve">need to decide a habitat and restoration measure OR a trajectory of restoration or improved management  </t>
   </si>
   <si>
+    <t>improved wetland management</t>
+  </si>
+  <si>
     <t>11,000 acres of wetland GDEs</t>
   </si>
   <si>
     <t>2025 = 38% of 2030 outcome</t>
   </si>
   <si>
+    <t>Baseline based on GSPs with HIGH (4+) scores in the SGMA Signals report (Fox Canyon - Oxnard, Fox Canyon Pleasant Valley and Grasslands); 2020 baseline based on GDE map; 2030 = 30 x 30 goal; implemented via SGMA implementation and based on other trend data outside of SGMA basins; assumes X% effectiveness</t>
+  </si>
+  <si>
+    <t>improved land management</t>
+  </si>
+  <si>
     <t>13,000 acres of vegetation GDEs</t>
   </si>
   <si>
+    <t>2020 baseline based on GSPs with HIGH (4+) scores in the SGMA Signals report (Fox Canyon - Oxnard, Fox Canyon Pleasant Valley and Grasslands); 2020 baseline based on GDE map; 2030 = 30 x 30 goal; implemented via SGMA implementation and based on other trend data outside of SGMA basins; assumes X% effectiveness</t>
+  </si>
+  <si>
     <t>112,000 acres/yr</t>
   </si>
   <si>
@@ -670,46 +712,7 @@
     <t xml:space="preserve">where strategy records JH did not populate 2025 outcome (groudwater sequestration/restoration wetland improved mgmt / avoid conversion) we calculated 2025 progress as 25% as per SM </t>
   </si>
   <si>
-    <t>crossing structures</t>
-  </si>
-  <si>
-    <t>decreased mortality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">avoided emissions and/or increased sequestration </t>
-  </si>
-  <si>
-    <t>within priority zones; of all actors; via influence, etc.</t>
-  </si>
-  <si>
-    <t>9 islands - California islands, double count with island biosec strategy</t>
-  </si>
-  <si>
-    <t>Baseline based on GSPs with HIGH (4+) scores in the SGMA Signals report (Fox Canyon - Oxnard, Fox Canyon Pleasant Valley and Grasslands); 2020 baseline based on GDE map; 2030 = 30 x 30 goal; implemented via SGMA implementation and based on other trend data outside of SGMA basins; assumes X% effectiveness</t>
-  </si>
-  <si>
-    <t>2020 baseline based on GSPs with HIGH (4+) scores in the SGMA Signals report (Fox Canyon - Oxnard, Fox Canyon Pleasant Valley and Grasslands); 2020 baseline based on GDE map; 2030 = 30 x 30 goal; implemented via SGMA implementation and based on other trend data outside of SGMA basins; assumes X% effectiveness</t>
-  </si>
-  <si>
-    <t>320K avoided CV lands and farmland via greenprints relative to BAU, assuming 75% effectiveness; plus 30K acres  via connected lands, assuming 25% effectiveness, Includes old Sus Dev strategy + disaster resilience - Carrie wrote methods doc</t>
-  </si>
-  <si>
-    <t>wildlife corridors and crossings</t>
-  </si>
-  <si>
-    <t>was 3 crossing structures in October 2021 metrics sheet, 2025 was originally 'designed and funded' changed to 1 structure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">note this is not TNC alone; climate emissions reduction; with some portion creditable to TNC- assumes a 58.8 MMTco2e 2019 emissions from electricity sector and linear decrease to 29 at 2030- cumulatively reduction relative to flat BAU </t>
-  </si>
-  <si>
-    <t>improved wetland management</t>
-  </si>
-  <si>
-    <t>improved land management</t>
-  </si>
-  <si>
-    <t>crossing structures designed and funded</t>
+    <t>8/30/22 Changed Forest strategy from Land to Climate program</t>
   </si>
   <si>
     <t>dynamic wetlands</t>
@@ -718,7 +721,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
@@ -1472,7 +1475,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25016BFA-BF6E-A048-A563-56E390B01DE9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A11:G37"/>
   <sheetViews>
     <sheetView topLeftCell="A21" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -1706,12 +1709,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B4D01AB-D785-4061-9828-98F183970D61}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1797,7 +1800,7 @@
         <v>48</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>212</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -1808,13 +1811,13 @@
         <v>43</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F3" s="54">
         <v>2025000</v>
@@ -1827,13 +1830,13 @@
         <v>6750420</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -1850,13 +1853,13 @@
         <v>42</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>213</v>
+        <v>56</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>218</v>
+        <v>57</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E5" s="14">
         <v>0</v>
@@ -1872,10 +1875,10 @@
         <v>2</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>205</v>
+        <v>59</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>214</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -1883,13 +1886,13 @@
         <v>42</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>213</v>
+        <v>56</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>206</v>
+        <v>61</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="56">
@@ -1903,7 +1906,7 @@
         <v>3</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>205</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -1917,16 +1920,16 @@
         <v>42</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="F8" s="54">
         <v>48000</v>
@@ -1942,10 +1945,10 @@
         <v>47</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -1953,13 +1956,13 @@
         <v>42</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E9" s="15">
         <v>0.33</v>
@@ -1975,13 +1978,13 @@
         <v>137000000</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>215</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -1995,16 +1998,16 @@
         <v>42</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>207</v>
+        <v>71</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="F11" s="54">
         <v>30000000</v>
@@ -2017,10 +2020,10 @@
         <v>100000000</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -2028,16 +2031,16 @@
         <v>42</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="F12" s="73">
         <v>6000000000</v>
@@ -2050,13 +2053,13 @@
         <v>10000000000</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="K12" s="13" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -2064,13 +2067,13 @@
         <v>42</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="57">
@@ -2087,156 +2090,156 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E14" s="28"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="58"/>
-    </row>
-    <row r="15" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="59">
-        <v>300000</v>
-      </c>
-      <c r="G15" s="38">
+    <row r="14" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="20"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="55"/>
+    </row>
+    <row r="15" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" s="54">
+        <v>1200000</v>
+      </c>
+      <c r="G15" s="15">
         <f>F15/H15</f>
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="H15" s="59">
-        <v>720000</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="J15" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="K15" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="59">
-        <v>400000</v>
-      </c>
-      <c r="G16" s="38">
+        <v>0.35294117647058826</v>
+      </c>
+      <c r="H15" s="54">
+        <v>3400000</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" s="73">
+        <v>625000</v>
+      </c>
+      <c r="G16" s="15">
         <f>F16/H16</f>
-        <v>0.51948051948051943</v>
-      </c>
-      <c r="H16" s="59">
-        <v>770000</v>
-      </c>
-      <c r="I16" s="10" t="s">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="H16" s="73">
+        <v>1125000</v>
+      </c>
+      <c r="I16" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="K16" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E17" s="22"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="60"/>
+      <c r="J16" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="28"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="58"/>
     </row>
     <row r="18" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>83</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="10"/>
       <c r="F18" s="59">
-        <v>1200000</v>
+        <v>300000</v>
       </c>
       <c r="G18" s="38">
         <f>F18/H18</f>
-        <v>0.35294117647058826</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="H18" s="59">
-        <v>3400000</v>
+        <v>720000</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>87</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="10"/>
       <c r="F19" s="59">
-        <v>625000</v>
+        <v>400000</v>
       </c>
       <c r="G19" s="38">
         <f>F19/H19</f>
-        <v>0.55555555555555558</v>
+        <v>0.51948051948051943</v>
       </c>
       <c r="H19" s="59">
-        <v>1125000</v>
+        <v>770000</v>
       </c>
       <c r="I19" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="J19" s="9" t="s">
-        <v>88</v>
+      <c r="J19" s="10" t="s">
+        <v>96</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -2247,19 +2250,19 @@
     </row>
     <row r="21" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F21" s="59">
         <v>150000</v>
@@ -2275,27 +2278,27 @@
         <v>47</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>208</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="F22" s="59">
         <v>135000</v>
@@ -2311,10 +2314,10 @@
         <v>47</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -2325,19 +2328,19 @@
     </row>
     <row r="24" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="F24" s="69">
         <v>185329</v>
@@ -2353,27 +2356,27 @@
         <v>47</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="F25" s="69">
         <v>15444086</v>
@@ -2389,10 +2392,10 @@
         <v>47</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -2403,19 +2406,19 @@
     </row>
     <row r="27" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="F27" s="69">
         <v>112000</v>
@@ -2431,27 +2434,27 @@
         <v>47</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="F28" s="69">
         <v>23750</v>
@@ -2467,10 +2470,10 @@
         <v>47</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>209</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -2481,19 +2484,19 @@
     </row>
     <row r="30" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B30" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D30" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>107</v>
-      </c>
       <c r="E30" s="8" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="F30" s="63">
         <v>150</v>
@@ -2509,27 +2512,27 @@
         <v>47</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B31" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D31" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>107</v>
-      </c>
       <c r="E31" s="8" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="F31" s="69">
         <v>16500</v>
@@ -2545,27 +2548,27 @@
         <v>47</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="K31" s="7" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="F32" s="74">
         <v>50000000</v>
@@ -2578,13 +2581,13 @@
         <v>200000000</v>
       </c>
       <c r="I32" s="32" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="K32" s="7" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -2595,19 +2598,19 @@
     </row>
     <row r="34" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="34" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B34" s="34" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="C34" s="34" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="F34" s="75">
         <v>0.125</v>
@@ -2620,30 +2623,30 @@
         <v>0.25</v>
       </c>
       <c r="I34" s="34" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="J34" s="34" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="K34" s="34" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="34" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B35" s="34" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="C35" s="34" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="D35" s="34" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="F35" s="64">
         <v>0.09</v>
@@ -2656,13 +2659,13 @@
         <v>0.9</v>
       </c>
       <c r="I35" s="35" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="J35" s="34" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="K35" s="34" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
     </row>
     <row r="36" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -2673,19 +2676,19 @@
     </row>
     <row r="37" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="F37" s="71">
         <v>300</v>
@@ -2698,28 +2701,28 @@
         <v>1000</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="J37" s="5"/>
       <c r="K37" s="4" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="F38" s="65">
         <v>15000</v>
@@ -2732,28 +2735,28 @@
         <v>33000</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="J38" s="5"/>
       <c r="K38" s="5" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="F39" s="71">
         <v>300</v>
@@ -2766,11 +2769,11 @@
         <v>1000</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="J39" s="5"/>
       <c r="K39" s="5" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
     </row>
     <row r="40" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -2781,19 +2784,19 @@
     </row>
     <row r="41" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="F41" s="65">
         <f xml:space="preserve"> H41*0.25</f>
@@ -2807,28 +2810,28 @@
         <v>237000000</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J41" s="5"/>
       <c r="K41" s="4" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="F42" s="71">
         <f>H42*0.25</f>
@@ -2845,24 +2848,24 @@
         <v>47</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="F43" s="67">
         <v>200000</v>
@@ -2878,27 +2881,27 @@
         <v>47</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
     </row>
     <row r="44" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>217</v>
+        <v>172</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E44" s="16" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="F44" s="67">
         <v>400000</v>
@@ -2915,7 +2918,7 @@
       </c>
       <c r="J44" s="6"/>
       <c r="K44" s="6" t="s">
-        <v>211</v>
+        <v>174</v>
       </c>
     </row>
     <row r="45" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -2926,19 +2929,19 @@
     </row>
     <row r="46" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="F46" s="71">
         <f>H46*0.25</f>
@@ -2956,24 +2959,24 @@
       </c>
       <c r="J46" s="5"/>
       <c r="K46" s="4" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
     </row>
     <row r="47" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="F47" s="71">
         <f>H47*0.25</f>
@@ -2991,11 +2994,11 @@
       </c>
       <c r="J47" s="5"/>
       <c r="K47" s="4" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A15:K22">
+  <sortState ref="A18:K22">
     <sortCondition ref="D1:D54"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3004,10 +3007,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{538B6C37-47B5-463B-A743-B7B49A4F65D8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -3050,10 +3053,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="C2" s="52">
         <f>CA_strategy_outcomes!F24</f>
@@ -3072,15 +3075,15 @@
         <v>300000.20677599998</v>
       </c>
       <c r="G2" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="C3" s="52">
         <f>(CA_strategy_outcomes!F25 + CA_strategy_outcomes!F30 + CA_strategy_outcomes!F31)</f>
@@ -3099,18 +3102,18 @@
         <v>25009532.07367</v>
       </c>
       <c r="G3" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="H3" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="F4" s="48"/>
     </row>
@@ -3126,50 +3129,50 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="E6" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="F6" s="48" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="F7" s="48" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="C8" s="48">
         <f>(CA_strategy_outcomes!F43 + CA_strategy_outcomes!F47)</f>
@@ -3188,15 +3191,15 @@
         <v>230266.334</v>
       </c>
       <c r="G8" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="C9" s="48">
         <f>(CA_strategy_outcomes!F37 + CA_strategy_outcomes!F38)</f>
@@ -3215,15 +3218,15 @@
         <v>54706</v>
       </c>
       <c r="G9" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="C10" s="48">
         <f>CA_strategy_outcomes!F46</f>
@@ -3242,15 +3245,15 @@
         <v>45324.832000000002</v>
       </c>
       <c r="G10" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="C11" s="48">
         <f>CA_strategy_outcomes!F39</f>
@@ -3269,7 +3272,7 @@
         <v>1609</v>
       </c>
       <c r="G11" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -3284,10 +3287,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="C13" s="52">
         <f>(CA_strategy_outcomes!F21 + CA_strategy_outcomes!F22)</f>
@@ -3306,18 +3309,18 @@
         <v>291373.92</v>
       </c>
       <c r="G13" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="C14" s="52">
-        <f>(CA_strategy_outcomes!F18 + CA_strategy_outcomes!F19 + CA_strategy_outcomes!F16 + CA_strategy_outcomes!F42 + CA_strategy_outcomes!F44 + CA_strategy_outcomes!F13 + CA_strategy_outcomes!F27)</f>
+        <f>(CA_strategy_outcomes!F15 + CA_strategy_outcomes!F16 + CA_strategy_outcomes!F19 + CA_strategy_outcomes!F42 + CA_strategy_outcomes!F44 + CA_strategy_outcomes!F13 + CA_strategy_outcomes!F27)</f>
         <v>2767300</v>
       </c>
       <c r="D14" s="49">
@@ -3325,7 +3328,7 @@
         <v>0.42277384127915324</v>
       </c>
       <c r="E14" s="52">
-        <f>(CA_strategy_outcomes!H18 + CA_strategy_outcomes!H19 + CA_strategy_outcomes!H16 + CA_strategy_outcomes!H42 + CA_strategy_outcomes!H44 + CA_strategy_outcomes!H13 + CA_strategy_outcomes!H27)</f>
+        <f>(CA_strategy_outcomes!H15 + CA_strategy_outcomes!H16 + CA_strategy_outcomes!H19 + CA_strategy_outcomes!H42 + CA_strategy_outcomes!H44 + CA_strategy_outcomes!H13 + CA_strategy_outcomes!H27)</f>
         <v>6545580</v>
       </c>
       <c r="F14" s="48">
@@ -3333,18 +3336,18 @@
         <v>2648904.58788</v>
       </c>
       <c r="G14" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="H14" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="C15" s="52">
         <f>(CA_strategy_outcomes!F2 + CA_strategy_outcomes!F8)</f>
@@ -3363,7 +3366,7 @@
         <v>206527.45324</v>
       </c>
       <c r="G15" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -3378,13 +3381,13 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="C17" s="48">
-        <f>(CA_strategy_outcomes!F3 + CA_strategy_outcomes!F9 + CA_strategy_outcomes!F11 + CA_strategy_outcomes!F15 + CA_strategy_outcomes!F141)</f>
+        <f>(CA_strategy_outcomes!F3 + CA_strategy_outcomes!F9 + CA_strategy_outcomes!F11 + CA_strategy_outcomes!F18 + CA_strategy_outcomes!F141)</f>
         <v>73425000</v>
       </c>
       <c r="D17" s="49">
@@ -3392,38 +3395,38 @@
         <v>0.3003430844516895</v>
       </c>
       <c r="E17" s="48">
-        <f>(CA_strategy_outcomes!H3 + CA_strategy_outcomes!H9 + CA_strategy_outcomes!H11 + CA_strategy_outcomes!H15 + CA_strategy_outcomes!H141)</f>
+        <f>(CA_strategy_outcomes!H3 + CA_strategy_outcomes!H9 + CA_strategy_outcomes!H11 + CA_strategy_outcomes!H18 + CA_strategy_outcomes!H141)</f>
         <v>244470420</v>
       </c>
       <c r="F17" s="48">
-        <f>(CA_strategy_outcomes!H3 + CA_strategy_outcomes!H9 + CA_strategy_outcomes!H11 + CA_strategy_outcomes!H15 + CA_strategy_outcomes!H141)</f>
+        <f>(CA_strategy_outcomes!H3 + CA_strategy_outcomes!H9 + CA_strategy_outcomes!H11 + CA_strategy_outcomes!H18 + CA_strategy_outcomes!H141)</f>
         <v>244470420</v>
       </c>
       <c r="G17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H17" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="C18" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="D18" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="E18" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="F18" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -3436,11 +3439,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8DD38FB-EBE8-2149-B921-33A0FF2374F4}">
-  <dimension ref="A1:B20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3458,45 +3461,45 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -3504,48 +3507,56 @@
         <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>199</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B16" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="B19" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>204</v>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>